<commit_message>
Extend the final table.
</commit_message>
<xml_diff>
--- a/Final Table.xlsx
+++ b/Final Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40140" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="40140" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="V16" authorId="0">
+    <comment ref="V19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -301,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -350,6 +350,10 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,7 +380,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -683,16 +687,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V969"/>
+  <dimension ref="A1:V972"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="30.5" customWidth="1"/>
-    <col min="2" max="17" width="4.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="4.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="4.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.1640625" bestFit="1" customWidth="1"/>
@@ -761,324 +768,246 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="8">
-        <v>0.25465838509299998</v>
-      </c>
-      <c r="C2" s="10">
-        <v>0.15</v>
-      </c>
-      <c r="D2" s="8">
-        <v>0.22368421052599999</v>
-      </c>
-      <c r="E2" s="8">
-        <v>8.3333333333299994E-2</v>
-      </c>
-      <c r="F2" s="10">
-        <v>0.28125</v>
-      </c>
-      <c r="G2" s="10">
-        <v>0.32098765432100002</v>
-      </c>
-      <c r="H2" s="8">
-        <v>6.9767441860500004E-2</v>
-      </c>
-      <c r="I2" s="10">
-        <v>0.222222222222</v>
-      </c>
-      <c r="J2" s="10">
-        <v>0.37614678899100001</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.16578947368399999</v>
-      </c>
-      <c r="L2" s="8">
-        <v>0.23404255319100001</v>
-      </c>
-      <c r="M2" s="8">
-        <v>9.67741935484E-2</v>
-      </c>
-      <c r="N2" s="8">
-        <v>5.6737588652499997E-2</v>
-      </c>
-      <c r="O2" s="17">
-        <v>8.8888888888899995E-2</v>
-      </c>
-      <c r="P2" s="10">
-        <v>0.103896103896</v>
-      </c>
-      <c r="Q2" s="10">
-        <v>8.8465845464700002E-2</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="13">
-        <f>AVERAGE(B2:Q2)</f>
-        <v>0.17604029272951877</v>
-      </c>
+    <row r="2" spans="1:22" s="15" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="16"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="10">
-        <v>0.30434782608700001</v>
-      </c>
-      <c r="G3" s="10">
-        <v>0.88888888888899997</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0.14285714285699999</v>
-      </c>
-      <c r="I3" s="10">
+        <v>60</v>
+      </c>
+      <c r="B3" s="7">
+        <f>AVERAGE(B7:B12)</f>
+        <v>0.25007986838433333</v>
+      </c>
+      <c r="C3" s="7">
+        <f>AVERAGE(C7:C12)</f>
+        <v>0.17488778765088001</v>
+      </c>
+      <c r="D3" s="7">
+        <f>AVERAGE(D7:D12)</f>
+        <v>0.28013496892083328</v>
+      </c>
+      <c r="E3" s="7">
+        <f>AVERAGE(E7:E12)</f>
+        <v>0.27833333333325</v>
+      </c>
+      <c r="F3" s="7">
+        <f>AVERAGE(F7:F12)</f>
+        <v>0.27736006683366665</v>
+      </c>
+      <c r="G3" s="7">
+        <f>AVERAGE(G7:G12)</f>
+        <v>0.47171191840325</v>
+      </c>
+      <c r="H3" s="7">
+        <f>AVERAGE(H7:H12)</f>
+        <v>0.33075242432625002</v>
+      </c>
+      <c r="I3" s="7">
+        <f>AVERAGE(I7:I12)</f>
+        <v>0.16689560439548334</v>
+      </c>
+      <c r="J3" s="7">
+        <f>AVERAGE(J7:J12)</f>
+        <v>0.11560029417175</v>
+      </c>
+      <c r="K3" s="7">
+        <f>AVERAGE(K7:K12)</f>
+        <v>0.32490810359220001</v>
+      </c>
+      <c r="L3" s="7">
+        <f>AVERAGE(L7:L12)</f>
         <v>0.26666666666700001</v>
       </c>
-      <c r="J3" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0.08</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="8">
-        <v>7.1428571428599999E-2</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="17">
-        <v>0.57142857142900005</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" s="10">
-        <v>0.26923076923099998</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" s="13">
-        <f>AVERAGE(B3:Q3)</f>
-        <v>0.33948484365886006</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="8">
-        <v>0.17307692307700001</v>
-      </c>
-      <c r="C4" s="10">
-        <v>5.2631578947399997E-2</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0.219178082192</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0.4375</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0.41095890411000002</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="18">
-        <v>5.7142857142900003E-2</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0.13333333333299999</v>
-      </c>
-      <c r="K4" s="8">
-        <v>0.23809523809499999</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" s="17">
-        <v>0.166666666667</v>
-      </c>
-      <c r="P4" s="10">
-        <v>0.1875</v>
-      </c>
-      <c r="Q4" s="10">
-        <v>0.31707317073199998</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U4" s="13">
-        <f>AVERAGE(B4:Q4)</f>
-        <v>0.21755970493602728</v>
-      </c>
+      <c r="M3" s="7">
+        <f>AVERAGE(M7:M12)</f>
+        <v>0.33715277777766667</v>
+      </c>
+      <c r="N3" s="7">
+        <f>AVERAGE(N7:N12)</f>
+        <v>0.532634032634</v>
+      </c>
+      <c r="O3" s="7">
+        <f>AVERAGE(O7:O12)</f>
+        <v>0.11386611241272501</v>
+      </c>
+      <c r="P3" s="7">
+        <f>AVERAGE(P7:P12)</f>
+        <v>0.267905169582</v>
+      </c>
+      <c r="Q3" s="7">
+        <f>AVERAGE(Q7:Q12)</f>
+        <v>0.320232329195</v>
+      </c>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:22" s="15" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="16"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B5" s="8">
-        <v>0.26666666666700001</v>
+        <v>0.25465838509299998</v>
       </c>
       <c r="C5" s="10">
-        <v>0.23809523809499999</v>
+        <v>0.15</v>
       </c>
       <c r="D5" s="8">
-        <v>0.36363636363599999</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>21</v>
+        <v>0.22368421052599999</v>
+      </c>
+      <c r="E5" s="8">
+        <v>8.3333333333299994E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.28125</v>
       </c>
       <c r="G5" s="10">
-        <v>0.402597402597</v>
+        <v>0.32098765432100002</v>
       </c>
       <c r="H5" s="8">
-        <v>0.41584158415799999</v>
-      </c>
-      <c r="I5" s="18">
-        <v>0.125</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>21</v>
+        <v>6.9767441860500004E-2</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.222222222222</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.37614678899100001</v>
       </c>
       <c r="K5" s="8">
-        <v>0.41269841269800001</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>21</v>
+        <v>0.16578947368399999</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0.23404255319100001</v>
       </c>
       <c r="M5" s="8">
-        <v>0.33333333333300003</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>21</v>
+        <v>9.67741935484E-2</v>
+      </c>
+      <c r="N5" s="8">
+        <v>5.6737588652499997E-2</v>
       </c>
       <c r="O5" s="17">
-        <v>0.13953488372100001</v>
+        <v>8.8888888888899995E-2</v>
       </c>
       <c r="P5" s="10">
-        <v>0.222222222222</v>
+        <v>0.103896103896</v>
       </c>
       <c r="Q5" s="10">
-        <v>0.35714285714299998</v>
+        <v>8.8465845464700002E-2</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="S5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="U5" s="13">
         <f>AVERAGE(B5:Q5)</f>
-        <v>0.29788808766090913</v>
+        <v>0.17604029272951877</v>
+      </c>
+      <c r="V5">
+        <f>COUNTIF(B5:Q5,"&gt;0")</f>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.29166666666699997</v>
+        <v>44</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="10">
-        <v>0.23749999999999999</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0.29411764705900001</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0.33333333333300003</v>
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="F6" s="10">
-        <v>0.428571428571</v>
+        <v>0.30434782608700001</v>
       </c>
       <c r="G6" s="10">
-        <v>0.5625</v>
+        <v>0.88888888888899997</v>
       </c>
       <c r="H6" s="8">
-        <v>0.39344262295100002</v>
+        <v>0.14285714285699999</v>
       </c>
       <c r="I6" s="10">
-        <v>0.05</v>
+        <v>0.26666666666700001</v>
       </c>
       <c r="J6" s="10">
-        <v>2.7027027027000002E-2</v>
+        <v>0.6</v>
       </c>
       <c r="K6" s="8">
-        <v>0.33684210526300001</v>
-      </c>
-      <c r="L6" s="8">
-        <v>0.26666666666700001</v>
+        <v>0.08</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="M6" s="8">
-        <v>0.328125</v>
-      </c>
-      <c r="N6" s="8">
-        <v>0.73076923076900002</v>
+        <v>7.1428571428599999E-2</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="O6" s="17">
-        <v>6.8181818181799997E-2</v>
-      </c>
-      <c r="P6" s="10">
-        <v>0.22727272727299999</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>21</v>
+        <v>0.57142857142900005</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>0.26923076923099998</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>23</v>
@@ -1088,129 +1017,137 @@
       </c>
       <c r="U6" s="13">
         <f>AVERAGE(B6:Q6)</f>
-        <v>0.30506775158411997</v>
+        <v>0.33948484365886006</v>
+      </c>
+      <c r="V6">
+        <f>COUNTIF(B6:Q6,"&gt;0")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B7" s="8">
-        <v>0.239130434783</v>
+        <v>0.17307692307700001</v>
       </c>
       <c r="C7" s="10">
-        <v>0.12121212121200001</v>
+        <v>5.2631578947399997E-2</v>
       </c>
       <c r="D7" s="8">
-        <v>0.258064516129</v>
+        <v>0.219178082192</v>
       </c>
       <c r="E7" s="8">
-        <v>6.25E-2</v>
+        <v>0.4375</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="10">
-        <v>0.51079136690600002</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0.34705882352900003</v>
-      </c>
-      <c r="I7" s="10">
-        <v>0.30769230769200001</v>
+        <v>0.41095890411000002</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="18">
+        <v>5.7142857142900003E-2</v>
       </c>
       <c r="J7" s="10">
-        <v>0.2</v>
+        <v>0.13333333333299999</v>
       </c>
       <c r="K7" s="8">
-        <v>0.26190476190500001</v>
-      </c>
-      <c r="L7" s="8">
-        <v>0.26666666666700001</v>
-      </c>
-      <c r="M7" s="8">
-        <v>0.35</v>
-      </c>
-      <c r="N7" s="8">
-        <v>0.73076923076900002</v>
+        <v>0.23809523809499999</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="O7" s="17">
-        <v>8.1081081081100001E-2</v>
+        <v>0.166666666667</v>
       </c>
       <c r="P7" s="10">
-        <v>0.121951219512</v>
+        <v>0.1875</v>
       </c>
       <c r="Q7" s="10">
-        <v>0.43478260869599999</v>
+        <v>0.31707317073199998</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="U7" s="13">
         <f>AVERAGE(B7:Q7)</f>
-        <v>0.28624034259207332</v>
+        <v>0.21755970493602728</v>
+      </c>
+      <c r="V7">
+        <f>COUNTIF(B7:Q7,"&gt;0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B8" s="8">
-        <v>0.25862068965500001</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>21</v>
+        <v>0.26666666666700001</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.23809523809499999</v>
       </c>
       <c r="D8" s="8">
-        <v>0.27407407407399997</v>
+        <v>0.36363636363599999</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="10">
-        <v>0.166666666667</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>21</v>
+      <c r="F8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.402597402597</v>
       </c>
       <c r="H8" s="8">
-        <v>0.166666666667</v>
-      </c>
-      <c r="I8" s="10">
-        <v>0.23076923076899999</v>
+        <v>0.41584158415799999</v>
+      </c>
+      <c r="I8" s="18">
+        <v>0.125</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>21</v>
+      <c r="K8" s="8">
+        <v>0.41269841269800001</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="7" t="s">
-        <v>21</v>
+      <c r="M8" s="8">
+        <v>0.33333333333300003</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="7" t="s">
-        <v>21</v>
+      <c r="O8" s="17">
+        <v>0.13953488372100001</v>
       </c>
       <c r="P8" s="10">
-        <v>0.181818181818</v>
+        <v>0.222222222222</v>
       </c>
       <c r="Q8" s="10">
-        <v>0.181818181818</v>
+        <v>0.35714285714299998</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>24</v>
@@ -1220,188 +1157,292 @@
       </c>
       <c r="U8" s="13">
         <f>AVERAGE(B8:Q8)</f>
-        <v>0.20863338449542859</v>
+        <v>0.29788808766090913</v>
+      </c>
+      <c r="V8">
+        <f>COUNTIF(B8:Q8,"&gt;0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B9" s="8">
-        <v>0.271317829457</v>
+        <v>0.29166666666699997</v>
       </c>
       <c r="C9" s="10">
-        <v>0.22500000000000001</v>
+        <v>0.23749999999999999</v>
       </c>
       <c r="D9" s="8">
-        <v>0.27173913043499998</v>
+        <v>0.29411764705900001</v>
       </c>
       <c r="E9" s="8">
-        <v>0.28000000000000003</v>
+        <v>0.33333333333300003</v>
       </c>
       <c r="F9" s="10">
-        <v>0.23684210526300001</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>21</v>
+        <v>0.428571428571</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0.39344262295100002</v>
       </c>
       <c r="I9" s="10">
-        <v>0.23076923076899999</v>
+        <v>0.05</v>
       </c>
       <c r="J9" s="10">
-        <v>0.102040816327</v>
+        <v>2.7027027027000002E-2</v>
       </c>
       <c r="K9" s="8">
-        <v>0.375</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>21</v>
+        <v>0.33684210526300001</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0.26666666666700001</v>
+      </c>
+      <c r="M9" s="8">
+        <v>0.328125</v>
       </c>
       <c r="N9" s="8">
-        <v>0.13636363636400001</v>
-      </c>
-      <c r="O9" s="19" t="s">
-        <v>21</v>
+        <v>0.73076923076900002</v>
+      </c>
+      <c r="O9" s="17">
+        <v>6.8181818181799997E-2</v>
       </c>
       <c r="P9" s="10">
-        <v>0.66666666666700003</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>0.31034482758600002</v>
+        <v>0.22727272727299999</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="S9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="U9" s="13">
         <f>AVERAGE(B9:Q9)</f>
-        <v>0.28237129480618184</v>
+        <v>0.30506775158411997</v>
+      </c>
+      <c r="V9">
+        <f>COUNTIF(B9:Q9,"&gt;0")</f>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="7"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
+      <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.239130434783</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.12121212121200001</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.258064516129</v>
+      </c>
+      <c r="E10" s="8">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.51079136690600002</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0.34705882352900003</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0.30769230769200001</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0.26190476190500001</v>
+      </c>
+      <c r="L10" s="8">
+        <v>0.26666666666700001</v>
+      </c>
+      <c r="M10" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="N10" s="8">
+        <v>0.73076923076900002</v>
+      </c>
+      <c r="O10" s="17">
+        <v>8.1081081081100001E-2</v>
+      </c>
+      <c r="P10" s="10">
+        <v>0.121951219512</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>0.43478260869599999</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U10" s="13">
+        <f>AVERAGE(B10:Q10)</f>
+        <v>0.28624034259207332</v>
+      </c>
+      <c r="V10">
+        <f>COUNTIF(B10:Q10,"&gt;0")</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="7">
-        <f>AVERAGE(B4:B9)</f>
-        <v>0.25007986838433333</v>
-      </c>
-      <c r="C11" s="7">
-        <f>AVERAGE(C4:C9)</f>
-        <v>0.17488778765088001</v>
-      </c>
-      <c r="D11" s="7">
-        <f>AVERAGE(D4:D9)</f>
-        <v>0.28013496892083328</v>
-      </c>
-      <c r="E11" s="7">
-        <f>AVERAGE(E4:E9)</f>
-        <v>0.27833333333325</v>
-      </c>
-      <c r="F11" s="7">
-        <f>AVERAGE(F4:F9)</f>
-        <v>0.27736006683366665</v>
-      </c>
-      <c r="G11" s="7">
-        <f>AVERAGE(G4:G9)</f>
-        <v>0.47171191840325</v>
-      </c>
-      <c r="H11" s="7">
-        <f>AVERAGE(H4:H9)</f>
-        <v>0.33075242432625002</v>
-      </c>
-      <c r="I11" s="7">
-        <f>AVERAGE(I4:I9)</f>
-        <v>0.16689560439548334</v>
-      </c>
-      <c r="J11" s="7">
-        <f>AVERAGE(J4:J9)</f>
-        <v>0.11560029417175</v>
-      </c>
-      <c r="K11" s="7">
-        <f>AVERAGE(K4:K9)</f>
-        <v>0.32490810359220001</v>
-      </c>
-      <c r="L11" s="7">
-        <f>AVERAGE(L4:L9)</f>
-        <v>0.26666666666700001</v>
-      </c>
-      <c r="M11" s="7">
-        <f>AVERAGE(M4:M9)</f>
-        <v>0.33715277777766667</v>
-      </c>
-      <c r="N11" s="7">
-        <f>AVERAGE(N4:N9)</f>
-        <v>0.532634032634</v>
-      </c>
-      <c r="O11" s="7">
-        <f>AVERAGE(O4:O9)</f>
-        <v>0.11386611241272501</v>
-      </c>
-      <c r="P11" s="7">
-        <f>AVERAGE(P4:P9)</f>
-        <v>0.267905169582</v>
-      </c>
-      <c r="Q11" s="7">
-        <f>AVERAGE(Q4:Q9)</f>
-        <v>0.320232329195</v>
-      </c>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.25862068965500001</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.27407407407399997</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.166666666667</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.166666666667</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.23076923076899999</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="10">
+        <v>0.181818181818</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>0.181818181818</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U11" s="13">
+        <f>AVERAGE(B11:Q11)</f>
+        <v>0.20863338449542859</v>
+      </c>
+      <c r="V11">
+        <f>COUNTIF(B11:Q11,"&gt;0")</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="7"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
+      <c r="A12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.271317829457</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.27173913043499998</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.23684210526300001</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0.23076923076899999</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0.102040816327</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" s="8">
+        <v>0.13636363636400001</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="10">
+        <v>0.66666666666700003</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>0.31034482758600002</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U12" s="13">
+        <f>AVERAGE(B12:Q12)</f>
+        <v>0.28237129480618184</v>
+      </c>
+      <c r="V12">
+        <f>COUNTIF(B12:Q12,"&gt;0")</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="7"/>
@@ -1424,146 +1465,34 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="8">
-        <v>7.1428571428599999E-2</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U14" s="13">
-        <f>AVERAGE(B14:Q14)</f>
-        <v>7.1428571428599999E-2</v>
-      </c>
-    </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="8">
-        <v>8.1632653061200003E-2</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q15" s="10">
-        <v>8.1911262798600004E-2</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U15" s="13">
-        <f>AVERAGE(B15:Q15)</f>
-        <v>8.1771957929899997E-2</v>
-      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -1574,14 +1503,13 @@
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="13"/>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>21</v>
@@ -1592,8 +1520,8 @@
       <c r="D17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>21</v>
+      <c r="E17" s="8">
+        <v>7.1428571428599999E-2</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>21</v>
@@ -1628,11 +1556,11 @@
       <c r="P17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q17" s="10">
-        <v>0.5</v>
+      <c r="Q17" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>23</v>
@@ -1642,24 +1570,28 @@
       </c>
       <c r="U17" s="13">
         <f>AVERAGE(B17:Q17)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>7.1428571428599999E-2</v>
+      </c>
+      <c r="V17">
+        <f>COUNTIF(B17:Q17,"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="10">
-        <v>0.166666666667</v>
+      <c r="C18" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="8">
-        <v>0.4375</v>
+        <v>8.1632653061200003E-2</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>21</v>
@@ -1676,14 +1608,14 @@
       <c r="J18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="8">
-        <v>0.14285714285699999</v>
+      <c r="K18" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="L18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="8">
-        <v>0.166666666667</v>
+      <c r="M18" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="N18" s="7" t="s">
         <v>21</v>
@@ -1694,170 +1626,135 @@
       <c r="P18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q18" s="7" t="s">
-        <v>21</v>
+      <c r="Q18" s="10">
+        <v>8.1911262798600004E-2</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="U18" s="13">
         <f>AVERAGE(B18:Q18)</f>
-        <v>0.22842261904775002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="10">
-        <v>0.15384615384600001</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q19" s="10">
-        <v>0.166666666667</v>
-      </c>
-      <c r="R19" s="1" t="s">
+        <v>8.1771957929899997E-2</v>
+      </c>
+      <c r="V18">
+        <f>COUNTIF(B18:Q18,"&gt;0")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="2"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="13"/>
+    </row>
+    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="S19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U19" s="13">
-        <f>AVERAGE(B19:Q19)</f>
-        <v>0.1602564102565</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="8">
-        <v>0.23809523809499999</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O20" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="P20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="R20" s="1" t="s">
+      <c r="S20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T20" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="U20" s="13">
         <f>AVERAGE(B20:Q20)</f>
-        <v>0.32936507936499998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.5</v>
+      </c>
+      <c r="V20">
+        <f>COUNTIF(B20:Q20,"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>21</v>
+      <c r="C21" s="10">
+        <v>0.166666666667</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>21</v>
+      <c r="E21" s="8">
+        <v>0.4375</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>21</v>
@@ -1874,14 +1771,14 @@
       <c r="J21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K21" s="7" t="s">
-        <v>21</v>
+      <c r="K21" s="8">
+        <v>0.14285714285699999</v>
       </c>
       <c r="L21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="7" t="s">
-        <v>21</v>
+      <c r="M21" s="8">
+        <v>0.166666666667</v>
       </c>
       <c r="N21" s="7" t="s">
         <v>21</v>
@@ -1892,11 +1789,11 @@
       <c r="P21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q21" s="10">
-        <v>0.5</v>
+      <c r="Q21" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>21</v>
@@ -1906,77 +1803,128 @@
       </c>
       <c r="U21" s="13">
         <f>AVERAGE(B21:Q21)</f>
+        <v>0.22842261904775002</v>
+      </c>
+      <c r="V21">
+        <f>COUNTIF(B21:Q21,"&gt;0")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0.15384615384600001</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22" s="10">
+        <v>0.166666666667</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U22" s="13">
+        <f>AVERAGE(B22:Q22)</f>
+        <v>0.1602564102565</v>
+      </c>
+      <c r="V22">
+        <f>COUNTIF(B22:Q22,"&gt;0")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0.23809523809499999</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="8">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="13"/>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0.33333333333300003</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M23" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O23" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="P23" s="7" t="s">
         <v>21</v>
@@ -1988,19 +1936,23 @@
         <v>24</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="U23" s="13">
         <f>AVERAGE(B23:Q23)</f>
-        <v>0.41666666666649999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.32936507936499998</v>
+      </c>
+      <c r="V23">
+        <f>COUNTIF(B23:Q23,"&gt;0")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>21</v>
@@ -2054,17 +2006,21 @@
         <v>24</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="U24" s="13">
         <f>AVERAGE(B24:Q24)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="V24">
+        <f>COUNTIF(B24:Q24,"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -2087,18 +2043,18 @@
       <c r="T25" s="1"/>
       <c r="U25" s="13"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="8">
-        <v>0.222222222222</v>
+        <v>36</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>21</v>
+      <c r="D26" s="8">
+        <v>0.33333333333300003</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>21</v>
@@ -2124,8 +2080,8 @@
       <c r="L26" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M26" s="7" t="s">
-        <v>21</v>
+      <c r="M26" s="8">
+        <v>0.5</v>
       </c>
       <c r="N26" s="7" t="s">
         <v>21</v>
@@ -2140,22 +2096,26 @@
         <v>21</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="T26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="U26" s="13">
         <f>AVERAGE(B26:Q26)</f>
-        <v>0.222222222222</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.41666666666649999</v>
+      </c>
+      <c r="V26">
+        <f>COUNTIF(B26:Q26,"&gt;0")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>21</v>
@@ -2166,8 +2126,8 @@
       <c r="D27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="8">
-        <v>0.4375</v>
+      <c r="E27" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>21</v>
@@ -2202,24 +2162,28 @@
       <c r="P27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q27" s="7" t="s">
-        <v>21</v>
+      <c r="Q27" s="10">
+        <v>0.5</v>
       </c>
       <c r="R27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="U27" s="13">
         <f>AVERAGE(B27:Q27)</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.5</v>
+      </c>
+      <c r="V27">
+        <f>COUNTIF(B27:Q27,"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -2242,12 +2206,12 @@
       <c r="T28" s="1"/>
       <c r="U28" s="13"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B29" s="8">
-        <v>0.33333333333300003</v>
+        <v>0.222222222222</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>21</v>
@@ -2294,308 +2258,281 @@
       <c r="Q29" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="T29" s="3" t="s">
-        <v>30</v>
+      <c r="R29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="U29" s="13">
         <f>AVERAGE(B29:Q29)</f>
+        <v>0.222222222222</v>
+      </c>
+      <c r="V29">
+        <f>COUNTIF(B29:Q29,"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0.4375</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U30" s="13">
+        <f>AVERAGE(B30:Q30)</f>
+        <v>0.4375</v>
+      </c>
+      <c r="V30">
+        <f>COUNTIF(B30:Q30,"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="2"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="13"/>
+    </row>
+    <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="8">
         <v>0.33333333333300003</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" ht="13" x14ac:dyDescent="0.15">
-      <c r="B30" s="7"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-    </row>
-    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="2" t="s">
+      <c r="C32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="U32" s="13">
+        <f>AVERAGE(B32:Q32)</f>
+        <v>0.33333333333300003</v>
+      </c>
+      <c r="V32">
+        <f>COUNTIF(B32:Q32,"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="13" x14ac:dyDescent="0.15">
+      <c r="B33" s="7"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+    </row>
+    <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" s="8">
+      <c r="B34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="8">
         <v>0.222222222222</v>
       </c>
-      <c r="N31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="R31" s="3" t="s">
+      <c r="N34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R34" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S31" s="3" t="s">
+      <c r="S34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T31" s="3" t="s">
+      <c r="T34" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="U31" s="13">
-        <f>AVERAGE(B31:Q31)</f>
-        <v>0.222222222222</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U32" s="13" t="e">
-        <f>AVERAGE(B32:Q32)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G33" s="10">
-        <v>0.35135135135099999</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M33" s="8">
-        <v>0.625</v>
-      </c>
-      <c r="N33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q33" s="10">
-        <v>0.36111111111100003</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U33" s="13">
-        <f>AVERAGE(B33:Q33)</f>
-        <v>0.44582082082066671</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="8">
-        <v>0.28571428571399998</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" s="10">
-        <v>0.43103448275900003</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S34" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="U34" s="13">
         <f>AVERAGE(B34:Q34)</f>
-        <v>0.35837438423650003</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.222222222222</v>
+      </c>
+      <c r="V34">
+        <f>COUNTIF(B34:Q34,"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>21</v>
@@ -2630,8 +2567,8 @@
       <c r="L35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M35" s="8">
-        <v>1</v>
+      <c r="M35" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="N35" s="7" t="s">
         <v>21</v>
@@ -2654,14 +2591,14 @@
       <c r="T35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="U35" s="13">
+      <c r="U35" s="13" t="e">
         <f>AVERAGE(B35:Q35)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>21</v>
@@ -2678,8 +2615,8 @@
       <c r="F36" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="9" t="s">
-        <v>21</v>
+      <c r="G36" s="10">
+        <v>0.35135135135099999</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>21</v>
@@ -2697,7 +2634,7 @@
         <v>21</v>
       </c>
       <c r="M36" s="8">
-        <v>1.5</v>
+        <v>0.625</v>
       </c>
       <c r="N36" s="7" t="s">
         <v>21</v>
@@ -2709,28 +2646,32 @@
         <v>21</v>
       </c>
       <c r="Q36" s="10">
-        <v>0.5</v>
+        <v>0.36111111111100003</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="S36" s="1" t="s">
         <v>23</v>
       </c>
       <c r="T36" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="U36" s="13">
         <f>AVERAGE(B36:Q36)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.44582082082066671</v>
+      </c>
+      <c r="V36">
+        <f>COUNTIF(B36:Q36,"&gt;0")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="B37" s="8">
+        <v>0.28571428571399998</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>21</v>
@@ -2744,8 +2685,8 @@
       <c r="F37" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G37" s="10">
-        <v>0.45454545454500001</v>
+      <c r="G37" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>21</v>
@@ -2753,8 +2694,8 @@
       <c r="I37" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J37" s="7" t="s">
-        <v>21</v>
+      <c r="J37" s="10">
+        <v>0.43103448275900003</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>21</v>
@@ -2774,11 +2715,11 @@
       <c r="P37" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q37" s="10">
-        <v>1</v>
+      <c r="Q37" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="S37" s="1" t="s">
         <v>23</v>
@@ -2788,12 +2729,16 @@
       </c>
       <c r="U37" s="13">
         <f>AVERAGE(B37:Q37)</f>
-        <v>0.72727272727250003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.35837438423650003</v>
+      </c>
+      <c r="V37">
+        <f>COUNTIF(B37:Q37,"&gt;0")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>21</v>
@@ -2828,8 +2773,8 @@
       <c r="L38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M38" s="7" t="s">
-        <v>21</v>
+      <c r="M38" s="8">
+        <v>1</v>
       </c>
       <c r="N38" s="7" t="s">
         <v>21</v>
@@ -2844,22 +2789,26 @@
         <v>21</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="T38" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U38" s="13" t="e">
+        <v>24</v>
+      </c>
+      <c r="U38" s="13">
         <f>AVERAGE(B38:Q38)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="V38">
+        <f>COUNTIF(B38:Q38,"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>21</v>
@@ -2894,8 +2843,8 @@
       <c r="L39" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M39" s="7" t="s">
-        <v>21</v>
+      <c r="M39" s="8">
+        <v>1.5</v>
       </c>
       <c r="N39" s="7" t="s">
         <v>21</v>
@@ -2906,8 +2855,8 @@
       <c r="P39" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q39" s="7" t="s">
-        <v>21</v>
+      <c r="Q39" s="10">
+        <v>0.5</v>
       </c>
       <c r="R39" s="1" t="s">
         <v>24</v>
@@ -2916,16 +2865,20 @@
         <v>23</v>
       </c>
       <c r="T39" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U39" s="13" t="e">
+        <v>24</v>
+      </c>
+      <c r="U39" s="13">
         <f>AVERAGE(B39:Q39)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="V39">
+        <f>COUNTIF(B39:Q39,"&gt;0")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>21</v>
@@ -2942,8 +2895,8 @@
       <c r="F40" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G40" s="9" t="s">
-        <v>21</v>
+      <c r="G40" s="10">
+        <v>0.45454545454500001</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>21</v>
@@ -2960,8 +2913,8 @@
       <c r="L40" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M40" s="8">
-        <v>1.2</v>
+      <c r="M40" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="N40" s="7" t="s">
         <v>21</v>
@@ -2973,7 +2926,7 @@
         <v>21</v>
       </c>
       <c r="Q40" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R40" s="1" t="s">
         <v>24</v>
@@ -2982,16 +2935,20 @@
         <v>23</v>
       </c>
       <c r="T40" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="U40" s="13">
         <f>AVERAGE(B40:Q40)</f>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.72727272727250003</v>
+      </c>
+      <c r="V40">
+        <f>COUNTIF(B40:Q40,"&gt;0")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>21</v>
@@ -3048,16 +3005,16 @@
         <v>21</v>
       </c>
       <c r="T41" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="U41" s="13" t="e">
         <f>AVERAGE(B41:Q41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>21</v>
@@ -3114,16 +3071,16 @@
         <v>23</v>
       </c>
       <c r="T42" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="U42" s="13" t="e">
         <f>AVERAGE(B42:Q42)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>21</v>
@@ -3159,7 +3116,7 @@
         <v>21</v>
       </c>
       <c r="M43" s="8">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="N43" s="7" t="s">
         <v>21</v>
@@ -3170,8 +3127,8 @@
       <c r="P43" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q43" s="7" t="s">
-        <v>21</v>
+      <c r="Q43" s="10">
+        <v>0.5</v>
       </c>
       <c r="R43" s="1" t="s">
         <v>24</v>
@@ -3184,73 +3141,216 @@
       </c>
       <c r="U43" s="13">
         <f>AVERAGE(B43:Q43)</f>
+        <v>0.85</v>
+      </c>
+      <c r="V43">
+        <f>COUNTIF(B43:Q43,"&gt;0")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U44" s="13" t="e">
+        <f>AVERAGE(B44:Q44)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U45" s="13" t="e">
+        <f>AVERAGE(B45:Q45)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M46" s="8">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" ht="13" x14ac:dyDescent="0.15">
-      <c r="B44" s="7"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-    </row>
-    <row r="45" spans="1:21" ht="13" x14ac:dyDescent="0.15">
-      <c r="B45" s="7"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="7"/>
-      <c r="Q45" s="7"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
-    </row>
-    <row r="46" spans="1:21" ht="13" x14ac:dyDescent="0.15">
-      <c r="B46" s="7"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
-      <c r="P46" s="7"/>
-      <c r="Q46" s="7"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-    </row>
-    <row r="47" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="N46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U46" s="13">
+        <f>AVERAGE(B46:Q46)</f>
+        <v>1.5</v>
+      </c>
+      <c r="V46">
+        <f>COUNTIF(B46:Q46,"&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="13" x14ac:dyDescent="0.15">
       <c r="B47" s="7"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
@@ -3271,26 +3371,74 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
     </row>
-    <row r="48" spans="1:21" ht="13" x14ac:dyDescent="0.15">
-      <c r="B48" s="7"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7"/>
-      <c r="P48" s="7"/>
-      <c r="Q48" s="7"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="3"/>
-      <c r="T48" s="3"/>
+    <row r="48" spans="1:22" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="B48" s="21">
+        <f>COUNTIF(B4:B46, "&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="C48" s="21">
+        <f>COUNTIF(C4:C46, "&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="D48" s="21">
+        <f>COUNTIF(D4:D46, "&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="E48" s="21">
+        <f>COUNTIF(E4:E46, "&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="F48" s="21">
+        <f>COUNTIF(F4:F46, "&gt;0")</f>
+        <v>6</v>
+      </c>
+      <c r="G48" s="21">
+        <f>COUNTIF(G4:G46, "&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="H48" s="21">
+        <f>COUNTIF(H4:H46, "&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="I48" s="21">
+        <f>COUNTIF(I4:I46, "&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="J48" s="21">
+        <f>COUNTIF(J4:J46, "&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="K48" s="21">
+        <f>COUNTIF(K4:K46, "&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="L48" s="21">
+        <f>COUNTIF(L4:L46, "&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="M48" s="21">
+        <f>COUNTIF(M4:M46, "&gt;0")</f>
+        <v>13</v>
+      </c>
+      <c r="N48" s="21">
+        <f>COUNTIF(N4:N46, "&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="O48" s="21">
+        <f>COUNTIF(O4:O46, "&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="P48" s="21">
+        <f>COUNTIF(P4:P46, "&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="Q48" s="21">
+        <f>COUNTIF(Q4:Q46, "&gt;0")</f>
+        <v>16</v>
+      </c>
+      <c r="R48" s="21"/>
+      <c r="S48" s="21"/>
+      <c r="T48" s="21"/>
     </row>
     <row r="49" spans="2:20" ht="13" x14ac:dyDescent="0.15">
       <c r="B49" s="7"/>
@@ -22633,6 +22781,69 @@
       <c r="S969" s="3"/>
       <c r="T969" s="3"/>
     </row>
+    <row r="970" spans="2:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="B970" s="7"/>
+      <c r="C970" s="11"/>
+      <c r="D970" s="11"/>
+      <c r="E970" s="7"/>
+      <c r="F970" s="7"/>
+      <c r="G970" s="7"/>
+      <c r="H970" s="7"/>
+      <c r="I970" s="7"/>
+      <c r="J970" s="7"/>
+      <c r="K970" s="7"/>
+      <c r="L970" s="7"/>
+      <c r="M970" s="7"/>
+      <c r="N970" s="7"/>
+      <c r="O970" s="7"/>
+      <c r="P970" s="7"/>
+      <c r="Q970" s="7"/>
+      <c r="R970" s="3"/>
+      <c r="S970" s="3"/>
+      <c r="T970" s="3"/>
+    </row>
+    <row r="971" spans="2:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="B971" s="7"/>
+      <c r="C971" s="11"/>
+      <c r="D971" s="11"/>
+      <c r="E971" s="7"/>
+      <c r="F971" s="7"/>
+      <c r="G971" s="7"/>
+      <c r="H971" s="7"/>
+      <c r="I971" s="7"/>
+      <c r="J971" s="7"/>
+      <c r="K971" s="7"/>
+      <c r="L971" s="7"/>
+      <c r="M971" s="7"/>
+      <c r="N971" s="7"/>
+      <c r="O971" s="7"/>
+      <c r="P971" s="7"/>
+      <c r="Q971" s="7"/>
+      <c r="R971" s="3"/>
+      <c r="S971" s="3"/>
+      <c r="T971" s="3"/>
+    </row>
+    <row r="972" spans="2:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="B972" s="7"/>
+      <c r="C972" s="11"/>
+      <c r="D972" s="11"/>
+      <c r="E972" s="7"/>
+      <c r="F972" s="7"/>
+      <c r="G972" s="7"/>
+      <c r="H972" s="7"/>
+      <c r="I972" s="7"/>
+      <c r="J972" s="7"/>
+      <c r="K972" s="7"/>
+      <c r="L972" s="7"/>
+      <c r="M972" s="7"/>
+      <c r="N972" s="7"/>
+      <c r="O972" s="7"/>
+      <c r="P972" s="7"/>
+      <c r="Q972" s="7"/>
+      <c r="R972" s="3"/>
+      <c r="S972" s="3"/>
+      <c r="T972" s="3"/>
+    </row>
   </sheetData>
   <sortState ref="A2:U11">
     <sortCondition ref="R2:R11"/>

</xml_diff>